<commit_message>
Correcion test case available Signed-off-by: qa-katalon <qa-katalon@DEV-QA-KatalonStudio.BMinc.eu>
</commit_message>
<xml_diff>
--- a/Data Files/TestData/Available hace match con informacion en CM (C6387).xlsx
+++ b/Data Files/TestData/Available hace match con informacion en CM (C6387).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="65">
   <si>
     <t xml:space="preserve">URL</t>
   </si>
@@ -203,6 +203,18 @@
   </si>
   <si>
     <t>10:46:34.613</t>
+  </si>
+  <si>
+    <t>17/10/2019</t>
+  </si>
+  <si>
+    <t>13:39:52.016</t>
+  </si>
+  <si>
+    <t>Firefox 69.0.3</t>
+  </si>
+  <si>
+    <t>13:40:45.020</t>
   </si>
 </sst>
 </file>
@@ -353,31 +365,31 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" t="s">
-        <v>58</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="E2" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="G2" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
       </c>
       <c r="I2" t="s">
-        <v>24</v>
+        <v>63</v>
       </c>
       <c r="J2" t="s">
         <v>26</v>

</xml_diff>